<commit_message>
Update 12/8/22 Building UI Database changes
</commit_message>
<xml_diff>
--- a/RavenDB/DataFiles/SystemData.xlsx
+++ b/RavenDB/DataFiles/SystemData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBeck\WorkDB\RLRMDB\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBeck\Raven\RavenDB\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78471FA-6A1C-477E-A70E-B56D619B81AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469C1C8-4270-4BDC-B0A8-167FE6968F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1836" yWindow="1452" windowWidth="18900" windowHeight="10248" activeTab="2" xr2:uid="{99EA2E09-E72F-4913-874B-0156ED8DAE70}"/>
+    <workbookView xWindow="0" yWindow="276" windowWidth="18900" windowHeight="10248" activeTab="1" xr2:uid="{99EA2E09-E72F-4913-874B-0156ED8DAE70}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Pressure!$A$1:$F$74</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Temp!$A$1:$F$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Temp!$B$1:$F$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="235">
   <si>
     <t>MaterialName</t>
   </si>
@@ -740,6 +740,12 @@
   </si>
   <si>
     <t>Reboiler Containment Pressure</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -1109,32 +1115,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12192771-724A-447B-B295-0DE083EBA54F}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:F50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1142,1403 +1150,1433 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10</v>
+        <v>93</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E2" s="1">
-        <v>20</v>
+        <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>225</v>
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="1">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="1">
+        <v>120</v>
+      </c>
       <c r="F3" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>234</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
+        <v>138</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="E4" s="1">
-        <v>20</v>
+        <v>175</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>201</v>
+        <v>234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="1">
-        <v>60</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-190</v>
+      </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>234</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="1">
-        <v>62</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="1">
+        <v>160</v>
+      </c>
       <c r="F6" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>234</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45</v>
+        <v>201</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="E7" s="1">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="1">
-        <v>105</v>
-      </c>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="1">
+        <v>62</v>
+      </c>
       <c r="F8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>234</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="1">
-        <v>61</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="1">
+        <v>105</v>
+      </c>
       <c r="F9" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D10" s="1">
-        <v>25</v>
+      <c r="D10" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E10" s="1">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="1">
-        <v>35</v>
+        <v>96</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="E11" s="1">
         <v>55</v>
       </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>234</v>
+      </c>
+      <c r="B12" t="s">
+        <v>149</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="1">
-        <v>55</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
       <c r="F12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>127</v>
+        <v>234</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="1">
-        <v>40</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30</v>
+      </c>
       <c r="F13" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="1">
-        <v>30</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="1">
+        <v>25</v>
+      </c>
       <c r="F14" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="1">
+        <v>190</v>
+      </c>
       <c r="F15" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>129</v>
+        <v>234</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="1">
-        <v>30</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="1">
+        <v>55</v>
+      </c>
       <c r="F16" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>223</v>
+        <v>234</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="1">
-        <v>30</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
       <c r="F17" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>125</v>
+        <v>234</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="1">
-        <v>27</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="1">
+        <v>145</v>
+      </c>
       <c r="F18" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="1">
-        <v>25</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" s="1">
+        <v>200</v>
+      </c>
       <c r="F19" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>127</v>
+        <v>234</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2</v>
+        <v>217</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="E20" s="1">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>129</v>
+        <v>234</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4</v>
+        <v>217</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="E21" s="1">
+        <v>195</v>
+      </c>
+      <c r="F21" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="1">
-        <v>45</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="1">
+        <v>130</v>
+      </c>
       <c r="F22" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>136</v>
+        <v>234</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="1">
-        <v>170</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="1">
+        <v>197</v>
+      </c>
       <c r="F23" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1">
         <v>140</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="1">
-        <v>190</v>
-      </c>
-      <c r="E24" s="1"/>
       <c r="F24" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>234</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" s="1">
-        <v>175</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="1">
+        <v>120</v>
+      </c>
       <c r="F25" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="1">
-        <v>55</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="1">
+        <v>120</v>
+      </c>
       <c r="F26" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B27" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" s="1">
-        <v>10</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="1">
+        <v>105</v>
+      </c>
       <c r="F27" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="1">
-        <v>-190</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="1">
+        <v>242</v>
+      </c>
       <c r="F28" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>216</v>
+        <v>234</v>
+      </c>
+      <c r="B29" t="s">
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D29" s="1">
-        <v>220</v>
+        <v>211</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="1">
+        <v>210</v>
       </c>
       <c r="F29" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>216</v>
+        <v>234</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="1">
-        <v>145</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="1">
+        <v>232</v>
+      </c>
       <c r="F30" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="1">
-        <v>200</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="1">
+        <v>205</v>
+      </c>
       <c r="F31" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>217</v>
+        <v>234</v>
+      </c>
+      <c r="B32" t="s">
+        <v>149</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="1">
-        <v>210</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>213</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" s="1">
+        <v>187</v>
+      </c>
       <c r="F32" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="1">
-        <v>130</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>225</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="1">
+        <v>25</v>
+      </c>
       <c r="F33" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>217</v>
+        <v>234</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" s="1">
-        <v>195</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="1">
+        <v>40</v>
+      </c>
       <c r="F34" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>218</v>
+        <v>234</v>
+      </c>
+      <c r="B35" t="s">
+        <v>111</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="1">
+        <v>129</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>43</v>
+      </c>
       <c r="F35" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>149</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>218</v>
+        <v>234</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D36" s="1">
-        <v>197</v>
+        <v>223</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="1">
+        <v>30</v>
       </c>
       <c r="F36" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>219</v>
+        <v>234</v>
+      </c>
+      <c r="B37" t="s">
+        <v>111</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="1">
-        <v>140</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="1">
+        <v>27</v>
+      </c>
       <c r="F37" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="1">
-        <v>120</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45</v>
+      </c>
       <c r="F38" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>221</v>
+        <v>234</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="1">
-        <v>120</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="1">
+        <v>170</v>
+      </c>
       <c r="F39" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>234</v>
+      </c>
+      <c r="B40" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="1">
-        <v>160</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" s="1">
+        <v>220</v>
+      </c>
       <c r="F40" s="1">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>234</v>
+      </c>
+      <c r="B41" t="s">
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="1">
-        <v>50</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>217</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="1">
+        <v>210</v>
+      </c>
       <c r="F41" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>149</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>234</v>
+      </c>
+      <c r="B42" t="s">
+        <v>168</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D42" s="1">
-        <v>120</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1">
-        <v>2</v>
+        <v>224</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="1">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>234</v>
+      </c>
+      <c r="B43" t="s">
         <v>168</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D43" s="1">
-        <v>20</v>
+        <v>225</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E43" s="1">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>149</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>158</v>
+        <v>234</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="1">
-        <v>105</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1">
+        <v>101</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="1">
+        <v>55</v>
+      </c>
+      <c r="F44">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>234</v>
+      </c>
+      <c r="B45" t="s">
         <v>168</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="1">
-        <v>4</v>
+        <v>99</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E45" s="1">
+        <v>35</v>
+      </c>
+      <c r="F45">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>111</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>211</v>
+        <v>234</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="1">
-        <v>242</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1">
+        <v>222</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E46" s="1">
+        <v>45</v>
+      </c>
+      <c r="F46">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>149</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>211</v>
+        <v>234</v>
+      </c>
+      <c r="B47" t="s">
+        <v>168</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" s="1">
-        <v>210</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1">
-        <v>10</v>
+        <v>127</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="F47">
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
+      </c>
+      <c r="B48" t="s">
+        <v>168</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="1">
-        <v>232</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1">
-        <v>10</v>
+        <v>129</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
+      </c>
+      <c r="B49" t="s">
+        <v>168</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D49" s="1">
-        <v>205</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1">
+        <v>158</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" s="1">
+        <v>30</v>
+      </c>
+      <c r="F49">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>213</v>
+        <v>234</v>
+      </c>
+      <c r="B50" t="s">
+        <v>168</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D50" s="1">
-        <v>187</v>
-      </c>
-      <c r="F50" s="1">
-        <v>10</v>
+        <v>177</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="1">
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="1"/>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="1"/>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="1"/>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="1"/>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="1"/>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="1"/>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="1"/>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="1"/>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="1"/>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" s="1"/>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B75" s="1"/>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="1"/>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="1"/>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B78" s="1"/>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="1"/>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="1"/>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" s="1"/>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="1"/>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B83" s="1"/>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B84" s="1"/>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B85" s="1"/>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B86" s="1"/>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B87" s="1"/>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="1"/>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="1"/>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B90" s="1"/>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="1"/>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B92" s="1"/>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B93" s="1"/>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B94" s="1"/>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B95" s="1"/>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="1"/>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="1"/>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="1"/>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B99" s="1"/>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="1"/>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="1"/>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B102" s="1"/>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B103" s="1"/>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="1"/>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="1"/>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B106" s="1"/>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B107" s="1"/>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B108" s="1"/>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B109" s="1"/>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B110" s="1"/>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B111" s="1"/>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B112" s="1"/>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B113" s="1"/>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B114" s="1"/>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B115" s="1"/>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B116" s="1"/>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B117" s="1"/>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B118" s="1"/>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B119" s="1"/>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B120" s="1"/>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B121" s="1"/>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B122" s="1"/>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B123" s="1"/>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B124" s="1"/>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B125" s="1"/>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B126" s="1"/>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B127" s="1"/>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F127" xr:uid="{12192771-724A-447B-B295-0DE083EBA54F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F127">
-      <sortCondition ref="B1:B127"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F125">
-    <sortCondition ref="A2:A125"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G127">
+    <sortCondition ref="F2:F127"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2550,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E78C427-8AD6-499F-A3F0-53D91B6643EF}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2822,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936D6970-3F83-4D5F-85C6-44505F4F7ADD}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>